<commit_message>
add ID_class conversion function
</commit_message>
<xml_diff>
--- a/roll_list.xlsx
+++ b/roll_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YLC/SynologyDrive/Code/Code_for_Exam/examprep/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YLC/Library/CloudStorage/SynologyDrive-YLC/myApp/examprep/examprep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5792303D-1E5B-584E-B5F6-D0DDFDD495C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9680BD-A4D3-1E47-AB6F-8CF3628E5ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="18980" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="18980" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>ID</t>
   </si>
@@ -28,13 +28,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>M120</t>
-  </si>
-  <si>
-    <t>甄艾完</t>
+    <t>甄任珍</t>
   </si>
 </sst>
 </file>
@@ -436,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -447,26 +441,20 @@
     <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>4070112345</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>